<commit_message>
Working on 'Postgres, Analiza anuala'
</commit_message>
<xml_diff>
--- a/Bundle/Ungheni/Deconectari/Analiza_anuala.xlsx
+++ b/Bundle/Ungheni/Deconectari/Analiza_anuala.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Red-Nord\07 Biroul dispecerului - PySide2_al_internet\Bundle\Ungheni\Deconectari\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frameworks\GitHub\Dispatcher_Bureau\Bundle\Ungheni\Deconectari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76CA46C-C7A6-46EA-8DDF-88C6FACC105F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4321094A-6B21-4CDF-A9C6-D9355285D908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A396AB9-6E7F-4978-AFCE-8C60F5766EE6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Programat" sheetId="1" r:id="rId1"/>
     <sheet name="Neprogramat" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="181029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,18 +31,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Ore</t>
   </si>
   <si>
-    <t>Nr. Consumatori</t>
-  </si>
-  <si>
     <t>PT, Fider</t>
   </si>
   <si>
     <t>Oficiul</t>
+  </si>
+  <si>
+    <t>Localitatea</t>
+  </si>
+  <si>
+    <t>Nr. Dec.</t>
+  </si>
+  <si>
+    <t>Nr. Cons.</t>
+  </si>
+  <si>
+    <t>Termen regl.</t>
   </si>
 </sst>
 </file>
@@ -464,28 +473,37 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="1"/>
     </row>
   </sheetData>
@@ -496,29 +514,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A424E49-8918-44E4-AF70-B96188F203CF}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>